<commit_message>
Adjust XLSX, circular ref and repairs
</commit_message>
<xml_diff>
--- a/app/public/CEM_template.xlsx
+++ b/app/public/CEM_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C913E9B0-9D7A-4E65-85A8-14FEE19F95DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD2740C0-13C7-45A6-9CFE-0B8342BE5EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="16200" tabRatio="719" xr2:uid="{9EB35D73-6E70-F94A-8F74-E60F0DF94BAF}"/>
+    <workbookView xWindow="1646" yWindow="9154" windowWidth="18720" windowHeight="12549" xr2:uid="{9EB35D73-6E70-F94A-8F74-E60F0DF94BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="5" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Cost Constants" sheetId="4" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -895,7 +896,7 @@
                   <c:v>44817161.003184728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44817161.003184728</c:v>
+                  <c:v>82405747.65101707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1473,7 +1474,7 @@
                   <c:v>38718004.158626646</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38718004.158626646</c:v>
+                  <c:v>76306590.806458995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3174,14 +3175,14 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.875" customWidth="1"/>
     <col min="2" max="2" width="42.625" customWidth="1"/>
@@ -3345,7 +3346,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{75B99312-59AF-4C4D-8D10-6BC2BBFAD1E0}"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{DC7DED59-414F-4590-84D1-E271CA32ECF3}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3364,7 +3365,7 @@
       <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3609,7 +3610,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
@@ -3643,7 +3644,7 @@
       <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
@@ -3717,7 +3718,7 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
@@ -3760,7 +3761,7 @@
       <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -3833,7 +3834,7 @@
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
   </cols>
@@ -3975,7 +3976,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5" customWidth="1"/>
   </cols>
@@ -4029,8 +4030,8 @@
         <v>5</v>
       </c>
       <c r="B6" s="18">
-        <f ca="1">'Yearly Values &amp; Costs'!B6-'Yearly Values &amp; Costs'!C6</f>
-        <v>38718004.158626646</v>
+        <f>'Yearly Values &amp; Costs'!B6-'Yearly Values &amp; Costs'!C6</f>
+        <v>76306590.806458995</v>
       </c>
     </row>
   </sheetData>
@@ -4053,11 +4054,11 @@
       <selection pane="bottomRight" activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,16 +4148,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f ca="1">'Portfolio Value Summary'!$G$23</f>
-        <v>44817161.003184728</v>
+        <f>'Portfolio Value Summary'!$G$23</f>
+        <v>82405747.65101707</v>
       </c>
       <c r="C6" s="1">
         <f>'Portfolio Cost Summary'!$G$13</f>
         <v>6099156.8445580788</v>
       </c>
       <c r="D6" s="16">
-        <f ca="1">B6-C6</f>
-        <v>38718004.158626646</v>
+        <f>B6-C6</f>
+        <v>76306590.806458995</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4175,14 +4176,14 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
       <selection pane="topRight" activeCell="M28" sqref="M28"/>
       <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.625" bestFit="1" customWidth="1"/>
@@ -4810,7 +4811,7 @@
         <v>44817161.003184728</v>
       </c>
       <c r="G23" s="11">
-        <f ca="1">SUM(C23:G23)</f>
+        <f>SUM(H9:H21)</f>
         <v>82405747.65101707</v>
       </c>
     </row>
@@ -4833,7 +4834,7 @@
       <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -5428,14 +5429,14 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
       <selection pane="topRight" activeCell="M28" sqref="M28"/>
       <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="31.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
@@ -5882,7 +5883,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
@@ -5920,7 +5921,7 @@
       <selection pane="bottomRight" activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
@@ -6166,7 +6167,7 @@
       <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>